<commit_message>
Add README, requirements, and citation file
</commit_message>
<xml_diff>
--- a/notebooks/evolving_sink_data_01.xlsx
+++ b/notebooks/evolving_sink_data_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hans-PeterSchmidt\Dropbox\Ithaka-Institute\Python\CH4-paper\notebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EACC958-F5F8-4BF9-9A8D-BBBBE34FC829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F742DB21-9041-49E2-AABA-0AD2E78FC884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{3D263A2E-BB47-4DAD-8D03-F02636E81219}"/>
   </bookViews>
@@ -416,7 +416,7 @@
   <dimension ref="A1:B102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -469,7 +469,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>-229.99999999999997</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -477,7 +477,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-219.99999999999997</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -485,7 +485,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-229.99999999999997</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -493,7 +493,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -501,7 +501,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>-330</v>
+        <v>-110</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -525,7 +525,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-409.99999999999994</v>
+        <v>-680</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -533,7 +533,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>-450</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -541,7 +541,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>-550</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -549,7 +549,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>-560</v>
+        <v>-300</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -573,7 +573,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>-710</v>
+        <v>-900</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -589,7 +589,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>-800</v>
+        <v>-400</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
@@ -597,7 +597,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>-830.00000000000011</v>
+        <v>-800</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">

</xml_diff>